<commit_message>
update templates, hide second 'Logging' sheet
</commit_message>
<xml_diff>
--- a/data/templates/template_timesheet_19_days.xlsx
+++ b/data/templates/template_timesheet_19_days.xlsx
@@ -5,10 +5,10 @@
   <workbookPr backupFile="false" showObjects="all" date1904="true"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Logging" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Logging" sheetId="1" state="hidden" r:id="rId2"/>
     <sheet name="Timesheet" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
@@ -293,42 +293,38 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -337,6 +333,10 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -361,16 +361,16 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="169" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -389,12 +389,12 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="171" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="171" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="171" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -409,20 +409,20 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="171" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="171" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -506,15 +506,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>63360</xdr:colOff>
+      <xdr:colOff>63720</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>178200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>152640</xdr:colOff>
+      <xdr:colOff>152280</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>191520</xdr:rowOff>
+      <xdr:rowOff>5400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -527,8 +527,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="332280" y="178200"/>
-          <a:ext cx="2476440" cy="1115640"/>
+          <a:off x="332640" y="178200"/>
+          <a:ext cx="2475720" cy="1114920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -551,7 +551,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -596,173 +596,173 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:M1048576"/>
+  <dimension ref="A1:M57"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J32" activeCellId="0" sqref="J32"/>
+      <selection pane="topLeft" activeCell="L10" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.65" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="18.45" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.61"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="4" style="0" width="10.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="8.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="10.07"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="23.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="3.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="14" style="0" width="10.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="3.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="11.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="4" style="1" width="10.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="8.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="10.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="23.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="3.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="14" style="1" width="10.94"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="21.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1"/>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-    </row>
-    <row r="2" customFormat="false" ht="21.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
-    </row>
-    <row r="3" customFormat="false" ht="21.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="1"/>
-      <c r="M3" s="1"/>
-    </row>
-    <row r="4" customFormat="false" ht="21.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="1"/>
-      <c r="M4" s="1"/>
-    </row>
-    <row r="5" customFormat="false" ht="21.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1"/>
-      <c r="B5" s="2" t="s">
+    <row r="1" customFormat="false" ht="25.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+    </row>
+    <row r="2" customFormat="false" ht="25.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+    </row>
+    <row r="3" customFormat="false" ht="25.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+    </row>
+    <row r="4" customFormat="false" ht="25.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+    </row>
+    <row r="5" customFormat="false" ht="25.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2"/>
+      <c r="B5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
-      <c r="L5" s="1"/>
-      <c r="M5" s="1"/>
-    </row>
-    <row r="6" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
-      <c r="L6" s="1"/>
-      <c r="M6" s="1"/>
-    </row>
-    <row r="7" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1"/>
-      <c r="B7" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+    </row>
+    <row r="6" customFormat="false" ht="18.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+    </row>
+    <row r="7" customFormat="false" ht="18.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
       <c r="C7" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
-      <c r="L7" s="1"/>
-      <c r="M7" s="1"/>
-    </row>
-    <row r="8" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1"/>
-      <c r="B8" s="3"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+    </row>
+    <row r="8" customFormat="false" ht="18.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
       <c r="C8" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="7" t="s">
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="I8" s="7"/>
-      <c r="J8" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="K8" s="8"/>
-      <c r="L8" s="1"/>
-      <c r="M8" s="1"/>
-    </row>
-    <row r="9" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
-      <c r="K9" s="1"/>
-      <c r="L9" s="1"/>
-      <c r="M9" s="1"/>
-    </row>
-    <row r="10" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1"/>
-      <c r="B10" s="3"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="K8" s="7"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+    </row>
+    <row r="9" customFormat="false" ht="18.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+    </row>
+    <row r="10" customFormat="false" ht="18.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
       <c r="C10" s="4" t="s">
         <v>7</v>
       </c>
@@ -788,28 +788,28 @@
         <v>14</v>
       </c>
       <c r="K10" s="4"/>
-      <c r="L10" s="9" t="s">
+      <c r="L10" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="M10" s="1"/>
-    </row>
-    <row r="11" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1"/>
-      <c r="B11" s="10"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="10"/>
-      <c r="I11" s="10"/>
-      <c r="J11" s="11"/>
-      <c r="K11" s="10"/>
-      <c r="L11" s="1"/>
-      <c r="M11" s="1"/>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1"/>
+      <c r="M10" s="2"/>
+    </row>
+    <row r="11" customFormat="false" ht="18.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="2"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="10"/>
+      <c r="K11" s="9"/>
+      <c r="L11" s="11"/>
+      <c r="M11" s="2"/>
+    </row>
+    <row r="12" customFormat="false" ht="18.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="2"/>
       <c r="B12" s="12"/>
       <c r="C12" s="13"/>
       <c r="D12" s="14"/>
@@ -830,10 +830,10 @@
       </c>
       <c r="K12" s="19"/>
       <c r="L12" s="20"/>
-      <c r="M12" s="1"/>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1"/>
+      <c r="M12" s="2"/>
+    </row>
+    <row r="13" customFormat="false" ht="18.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="2"/>
       <c r="B13" s="12"/>
       <c r="C13" s="13"/>
       <c r="D13" s="14"/>
@@ -854,10 +854,10 @@
       </c>
       <c r="K13" s="19"/>
       <c r="L13" s="20"/>
-      <c r="M13" s="1"/>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1"/>
+      <c r="M13" s="2"/>
+    </row>
+    <row r="14" customFormat="false" ht="18.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="2"/>
       <c r="B14" s="12"/>
       <c r="C14" s="13"/>
       <c r="D14" s="14"/>
@@ -878,10 +878,10 @@
       </c>
       <c r="K14" s="19"/>
       <c r="L14" s="20"/>
-      <c r="M14" s="1"/>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1"/>
+      <c r="M14" s="2"/>
+    </row>
+    <row r="15" customFormat="false" ht="18.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="2"/>
       <c r="B15" s="12"/>
       <c r="C15" s="13"/>
       <c r="D15" s="14"/>
@@ -902,10 +902,10 @@
       </c>
       <c r="K15" s="19"/>
       <c r="L15" s="20"/>
-      <c r="M15" s="1"/>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1"/>
+      <c r="M15" s="2"/>
+    </row>
+    <row r="16" customFormat="false" ht="18.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="2"/>
       <c r="B16" s="12"/>
       <c r="C16" s="13"/>
       <c r="D16" s="14"/>
@@ -926,10 +926,10 @@
       </c>
       <c r="K16" s="25"/>
       <c r="L16" s="20"/>
-      <c r="M16" s="1"/>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1"/>
+      <c r="M16" s="2"/>
+    </row>
+    <row r="17" customFormat="false" ht="18.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="2"/>
       <c r="B17" s="12"/>
       <c r="C17" s="13"/>
       <c r="D17" s="14"/>
@@ -950,10 +950,10 @@
       </c>
       <c r="K17" s="25"/>
       <c r="L17" s="20"/>
-      <c r="M17" s="1"/>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1"/>
+      <c r="M17" s="2"/>
+    </row>
+    <row r="18" customFormat="false" ht="18.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A18" s="2"/>
       <c r="B18" s="12"/>
       <c r="C18" s="13"/>
       <c r="D18" s="14"/>
@@ -974,10 +974,10 @@
       </c>
       <c r="K18" s="25"/>
       <c r="L18" s="20"/>
-      <c r="M18" s="1"/>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1"/>
+      <c r="M18" s="2"/>
+    </row>
+    <row r="19" customFormat="false" ht="18.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="2"/>
       <c r="B19" s="12"/>
       <c r="C19" s="13"/>
       <c r="D19" s="14"/>
@@ -998,10 +998,10 @@
       </c>
       <c r="K19" s="25"/>
       <c r="L19" s="20"/>
-      <c r="M19" s="1"/>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="1"/>
+      <c r="M19" s="2"/>
+    </row>
+    <row r="20" customFormat="false" ht="18.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="2"/>
       <c r="B20" s="12"/>
       <c r="C20" s="13"/>
       <c r="D20" s="14"/>
@@ -1022,10 +1022,10 @@
       </c>
       <c r="K20" s="25"/>
       <c r="L20" s="20"/>
-      <c r="M20" s="1"/>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="1"/>
+      <c r="M20" s="2"/>
+    </row>
+    <row r="21" customFormat="false" ht="18.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A21" s="2"/>
       <c r="B21" s="12"/>
       <c r="C21" s="13"/>
       <c r="D21" s="14"/>
@@ -1046,10 +1046,10 @@
       </c>
       <c r="K21" s="25"/>
       <c r="L21" s="20"/>
-      <c r="M21" s="1"/>
-    </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="1"/>
+      <c r="M21" s="2"/>
+    </row>
+    <row r="22" customFormat="false" ht="18.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A22" s="2"/>
       <c r="B22" s="12"/>
       <c r="C22" s="13"/>
       <c r="D22" s="14"/>
@@ -1070,10 +1070,10 @@
       </c>
       <c r="K22" s="25"/>
       <c r="L22" s="20"/>
-      <c r="M22" s="1"/>
-    </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="1"/>
+      <c r="M22" s="2"/>
+    </row>
+    <row r="23" customFormat="false" ht="18.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A23" s="2"/>
       <c r="B23" s="12"/>
       <c r="C23" s="13"/>
       <c r="D23" s="14"/>
@@ -1094,10 +1094,10 @@
       </c>
       <c r="K23" s="25"/>
       <c r="L23" s="20"/>
-      <c r="M23" s="1"/>
-    </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="1"/>
+      <c r="M23" s="2"/>
+    </row>
+    <row r="24" customFormat="false" ht="18.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A24" s="2"/>
       <c r="B24" s="12"/>
       <c r="C24" s="13"/>
       <c r="D24" s="14"/>
@@ -1118,10 +1118,10 @@
       </c>
       <c r="K24" s="25"/>
       <c r="L24" s="20"/>
-      <c r="M24" s="1"/>
-    </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="1"/>
+      <c r="M24" s="2"/>
+    </row>
+    <row r="25" customFormat="false" ht="18.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A25" s="2"/>
       <c r="B25" s="12"/>
       <c r="C25" s="13"/>
       <c r="D25" s="14"/>
@@ -1142,10 +1142,10 @@
       </c>
       <c r="K25" s="25"/>
       <c r="L25" s="20"/>
-      <c r="M25" s="1"/>
-    </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="1"/>
+      <c r="M25" s="2"/>
+    </row>
+    <row r="26" customFormat="false" ht="18.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A26" s="2"/>
       <c r="B26" s="12"/>
       <c r="C26" s="13"/>
       <c r="D26" s="14"/>
@@ -1166,10 +1166,10 @@
       </c>
       <c r="K26" s="25"/>
       <c r="L26" s="20"/>
-      <c r="M26" s="1"/>
-    </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="1"/>
+      <c r="M26" s="2"/>
+    </row>
+    <row r="27" customFormat="false" ht="18.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A27" s="2"/>
       <c r="B27" s="12"/>
       <c r="C27" s="13"/>
       <c r="D27" s="14"/>
@@ -1190,10 +1190,10 @@
       </c>
       <c r="K27" s="25"/>
       <c r="L27" s="20"/>
-      <c r="M27" s="1"/>
-    </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="1"/>
+      <c r="M27" s="2"/>
+    </row>
+    <row r="28" customFormat="false" ht="18.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A28" s="2"/>
       <c r="B28" s="12"/>
       <c r="C28" s="13"/>
       <c r="D28" s="14"/>
@@ -1214,10 +1214,10 @@
       </c>
       <c r="K28" s="25"/>
       <c r="L28" s="20"/>
-      <c r="M28" s="1"/>
-    </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="1"/>
+      <c r="M28" s="2"/>
+    </row>
+    <row r="29" customFormat="false" ht="18.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A29" s="2"/>
       <c r="B29" s="12"/>
       <c r="C29" s="13"/>
       <c r="D29" s="14"/>
@@ -1238,16 +1238,16 @@
       </c>
       <c r="K29" s="25"/>
       <c r="L29" s="20"/>
-      <c r="M29" s="1"/>
-    </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="1"/>
+      <c r="M29" s="2"/>
+    </row>
+    <row r="30" customFormat="false" ht="18.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A30" s="2"/>
       <c r="B30" s="12"/>
       <c r="C30" s="13"/>
       <c r="D30" s="14"/>
       <c r="E30" s="15"/>
-      <c r="F30" s="23"/>
-      <c r="G30" s="24"/>
+      <c r="F30" s="15"/>
+      <c r="G30" s="14"/>
       <c r="H30" s="22" t="n">
         <f aca="false">(HOUR(G30-F30)*60+(MINUTE(G30-F30)))/60</f>
         <v>0</v>
@@ -1262,91 +1262,91 @@
       </c>
       <c r="K30" s="25"/>
       <c r="L30" s="20"/>
-      <c r="M30" s="1"/>
-    </row>
-    <row r="31" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="1"/>
-      <c r="B31" s="3"/>
-      <c r="C31" s="3"/>
-      <c r="D31" s="3"/>
-      <c r="E31" s="3"/>
-      <c r="F31" s="3"/>
-      <c r="G31" s="3"/>
-      <c r="H31" s="1"/>
+      <c r="M30" s="2"/>
+    </row>
+    <row r="31" customFormat="false" ht="18.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A31" s="2"/>
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
+      <c r="H31" s="2"/>
       <c r="I31" s="26"/>
-      <c r="J31" s="1"/>
+      <c r="J31" s="2"/>
       <c r="K31" s="26"/>
-      <c r="L31" s="1"/>
-      <c r="M31" s="1"/>
-    </row>
-    <row r="32" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="1"/>
-      <c r="B32" s="3"/>
-      <c r="C32" s="6"/>
-      <c r="D32" s="6"/>
-      <c r="E32" s="6"/>
-      <c r="F32" s="6"/>
-      <c r="G32" s="6"/>
-      <c r="H32" s="7" t="s">
+      <c r="L31" s="2"/>
+      <c r="M31" s="2"/>
+    </row>
+    <row r="32" customFormat="false" ht="18.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A32" s="2"/>
+      <c r="B32" s="2"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="5"/>
+      <c r="G32" s="5"/>
+      <c r="H32" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="I32" s="7"/>
+      <c r="I32" s="6"/>
       <c r="J32" s="27" t="n">
         <f aca="false">I36-D36+J8</f>
         <v>-152</v>
       </c>
       <c r="K32" s="27"/>
-      <c r="L32" s="1"/>
-      <c r="M32" s="1"/>
-    </row>
-    <row r="33" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="1"/>
-      <c r="B33" s="3"/>
-      <c r="C33" s="3"/>
-      <c r="D33" s="3"/>
-      <c r="E33" s="3"/>
-      <c r="F33" s="3"/>
-      <c r="G33" s="3"/>
-      <c r="H33" s="1"/>
+      <c r="L32" s="2"/>
+      <c r="M32" s="2"/>
+    </row>
+    <row r="33" customFormat="false" ht="18.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A33" s="2"/>
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
+      <c r="G33" s="2"/>
+      <c r="H33" s="2"/>
       <c r="I33" s="26"/>
-      <c r="J33" s="1"/>
+      <c r="J33" s="2"/>
       <c r="K33" s="26"/>
-      <c r="L33" s="1"/>
-      <c r="M33" s="1"/>
-    </row>
-    <row r="34" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="1"/>
-      <c r="B34" s="3"/>
-      <c r="C34" s="3"/>
-      <c r="D34" s="3"/>
-      <c r="E34" s="3"/>
-      <c r="F34" s="3"/>
-      <c r="G34" s="3"/>
-      <c r="H34" s="1"/>
+      <c r="L33" s="2"/>
+      <c r="M33" s="2"/>
+    </row>
+    <row r="34" customFormat="false" ht="18.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A34" s="2"/>
+      <c r="B34" s="2"/>
+      <c r="C34" s="2"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2"/>
+      <c r="G34" s="2"/>
+      <c r="H34" s="2"/>
       <c r="I34" s="26"/>
-      <c r="J34" s="1"/>
+      <c r="J34" s="2"/>
       <c r="K34" s="26"/>
-      <c r="L34" s="1"/>
-      <c r="M34" s="1"/>
-    </row>
-    <row r="35" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="1"/>
-      <c r="B35" s="3"/>
-      <c r="C35" s="3"/>
-      <c r="D35" s="3"/>
-      <c r="E35" s="3"/>
-      <c r="F35" s="3"/>
-      <c r="G35" s="3"/>
-      <c r="H35" s="1"/>
+      <c r="L34" s="2"/>
+      <c r="M34" s="2"/>
+    </row>
+    <row r="35" customFormat="false" ht="18.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A35" s="2"/>
+      <c r="B35" s="2"/>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="2"/>
+      <c r="G35" s="2"/>
+      <c r="H35" s="2"/>
       <c r="I35" s="26"/>
-      <c r="J35" s="1"/>
+      <c r="J35" s="2"/>
       <c r="K35" s="26"/>
-      <c r="L35" s="1"/>
-      <c r="M35" s="1"/>
-    </row>
-    <row r="36" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="1"/>
-      <c r="B36" s="3"/>
+      <c r="L35" s="2"/>
+      <c r="M35" s="2"/>
+    </row>
+    <row r="36" customFormat="false" ht="18.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A36" s="2"/>
+      <c r="B36" s="2"/>
       <c r="C36" s="28" t="s">
         <v>16</v>
       </c>
@@ -1354,9 +1354,9 @@
         <f aca="false">ROWS(D12:D30)*8</f>
         <v>152</v>
       </c>
-      <c r="E36" s="3"/>
-      <c r="F36" s="3"/>
-      <c r="G36" s="3"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="2"/>
+      <c r="G36" s="2"/>
       <c r="H36" s="30" t="s">
         <v>17</v>
       </c>
@@ -1366,174 +1366,174 @@
       </c>
       <c r="J36" s="31"/>
       <c r="K36" s="32"/>
-      <c r="L36" s="1"/>
-      <c r="M36" s="1"/>
-    </row>
-    <row r="37" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="1"/>
-      <c r="B37" s="3"/>
-      <c r="C37" s="3"/>
-      <c r="D37" s="3"/>
-      <c r="E37" s="3"/>
-      <c r="F37" s="3"/>
-      <c r="G37" s="3"/>
-      <c r="H37" s="1"/>
-      <c r="I37" s="1"/>
-      <c r="J37" s="1"/>
+      <c r="L36" s="2"/>
+      <c r="M36" s="2"/>
+    </row>
+    <row r="37" customFormat="false" ht="18.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A37" s="2"/>
+      <c r="B37" s="2"/>
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
+      <c r="G37" s="2"/>
+      <c r="H37" s="2"/>
+      <c r="I37" s="2"/>
+      <c r="J37" s="2"/>
       <c r="K37" s="26"/>
-      <c r="L37" s="1"/>
-      <c r="M37" s="1"/>
-    </row>
-    <row r="38" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="1"/>
-      <c r="B38" s="1"/>
-      <c r="C38" s="1"/>
-      <c r="D38" s="1"/>
-      <c r="E38" s="1"/>
-      <c r="F38" s="1"/>
-      <c r="G38" s="1"/>
-      <c r="H38" s="1"/>
-      <c r="I38" s="1"/>
-      <c r="J38" s="1"/>
-      <c r="K38" s="1"/>
-      <c r="L38" s="1"/>
-      <c r="M38" s="1"/>
-    </row>
-    <row r="39" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="1"/>
-      <c r="B39" s="1"/>
-      <c r="C39" s="1" t="s">
+      <c r="L37" s="2"/>
+      <c r="M37" s="2"/>
+    </row>
+    <row r="38" customFormat="false" ht="18.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A38" s="2"/>
+      <c r="B38" s="2"/>
+      <c r="C38" s="2"/>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+      <c r="F38" s="2"/>
+      <c r="G38" s="2"/>
+      <c r="H38" s="2"/>
+      <c r="I38" s="2"/>
+      <c r="J38" s="2"/>
+      <c r="K38" s="2"/>
+      <c r="L38" s="2"/>
+      <c r="M38" s="2"/>
+    </row>
+    <row r="39" customFormat="false" ht="18.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A39" s="2"/>
+      <c r="B39" s="11"/>
+      <c r="C39" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="D39" s="1"/>
-      <c r="E39" s="1"/>
-      <c r="F39" s="1"/>
-      <c r="G39" s="1" t="s">
+      <c r="D39" s="11"/>
+      <c r="E39" s="11"/>
+      <c r="F39" s="11"/>
+      <c r="G39" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="H39" s="1"/>
-      <c r="I39" s="1"/>
-      <c r="J39" s="1"/>
-      <c r="K39" s="1" t="s">
+      <c r="H39" s="11"/>
+      <c r="I39" s="11"/>
+      <c r="J39" s="11"/>
+      <c r="K39" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="L39" s="1"/>
-      <c r="M39" s="1"/>
-    </row>
-    <row r="40" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="1"/>
-      <c r="B40" s="1"/>
-      <c r="C40" s="1"/>
-      <c r="D40" s="1"/>
-      <c r="E40" s="1"/>
-      <c r="F40" s="1"/>
-      <c r="G40" s="1"/>
-      <c r="H40" s="1"/>
-      <c r="I40" s="1"/>
-      <c r="J40" s="1"/>
-      <c r="K40" s="1"/>
-      <c r="L40" s="1"/>
-      <c r="M40" s="1"/>
-    </row>
-    <row r="41" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="1"/>
-      <c r="B41" s="1"/>
-      <c r="C41" s="1" t="s">
+      <c r="L39" s="11"/>
+      <c r="M39" s="2"/>
+    </row>
+    <row r="40" customFormat="false" ht="18.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A40" s="2"/>
+      <c r="B40" s="11"/>
+      <c r="C40" s="11"/>
+      <c r="D40" s="11"/>
+      <c r="E40" s="11"/>
+      <c r="F40" s="11"/>
+      <c r="G40" s="11"/>
+      <c r="H40" s="11"/>
+      <c r="I40" s="11"/>
+      <c r="J40" s="11"/>
+      <c r="K40" s="11"/>
+      <c r="L40" s="11"/>
+      <c r="M40" s="2"/>
+    </row>
+    <row r="41" customFormat="false" ht="18.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A41" s="2"/>
+      <c r="B41" s="2"/>
+      <c r="C41" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="D41" s="1"/>
-      <c r="E41" s="1"/>
-      <c r="F41" s="1"/>
-      <c r="G41" s="1" t="s">
+      <c r="D41" s="11"/>
+      <c r="E41" s="11"/>
+      <c r="F41" s="11"/>
+      <c r="G41" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="H41" s="1"/>
-      <c r="I41" s="1"/>
-      <c r="J41" s="1"/>
-      <c r="K41" s="1" t="s">
+      <c r="H41" s="11"/>
+      <c r="I41" s="11"/>
+      <c r="J41" s="11"/>
+      <c r="K41" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="L41" s="1"/>
-      <c r="M41" s="1"/>
-    </row>
-    <row r="42" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="1"/>
-      <c r="B42" s="1"/>
-      <c r="C42" s="1"/>
-      <c r="D42" s="1"/>
-      <c r="E42" s="1"/>
-      <c r="F42" s="1"/>
-      <c r="G42" s="1"/>
-      <c r="H42" s="1"/>
-      <c r="I42" s="1"/>
-      <c r="J42" s="1"/>
-      <c r="K42" s="1"/>
-      <c r="L42" s="1"/>
-      <c r="M42" s="1"/>
-    </row>
-    <row r="43" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="1"/>
-      <c r="B43" s="1"/>
-      <c r="C43" s="1"/>
-      <c r="D43" s="1"/>
-      <c r="E43" s="1"/>
-      <c r="F43" s="1"/>
-      <c r="G43" s="1"/>
-      <c r="H43" s="1"/>
-      <c r="I43" s="1"/>
-      <c r="J43" s="1"/>
-      <c r="K43" s="1"/>
-      <c r="L43" s="1"/>
-      <c r="M43" s="1"/>
-    </row>
-    <row r="44" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="1"/>
-      <c r="B44" s="1"/>
-      <c r="C44" s="1"/>
-      <c r="D44" s="1"/>
-      <c r="E44" s="1"/>
-      <c r="F44" s="1"/>
-      <c r="G44" s="1"/>
-      <c r="H44" s="1"/>
-      <c r="I44" s="1"/>
-      <c r="J44" s="1"/>
-      <c r="K44" s="1"/>
-      <c r="L44" s="1"/>
-      <c r="M44" s="1"/>
-    </row>
-    <row r="45" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="1"/>
-      <c r="B45" s="1"/>
-      <c r="C45" s="1"/>
-      <c r="D45" s="1"/>
-      <c r="E45" s="1"/>
-      <c r="F45" s="1"/>
-      <c r="G45" s="1"/>
-      <c r="H45" s="1"/>
-      <c r="I45" s="1"/>
-      <c r="J45" s="1"/>
-      <c r="K45" s="1"/>
-      <c r="L45" s="1"/>
-      <c r="M45" s="1"/>
-    </row>
-    <row r="46" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="1"/>
-      <c r="B46" s="1"/>
-      <c r="C46" s="1"/>
-      <c r="D46" s="1"/>
-      <c r="E46" s="1"/>
-      <c r="F46" s="1"/>
-      <c r="G46" s="1"/>
-      <c r="H46" s="1"/>
-      <c r="I46" s="1"/>
-      <c r="J46" s="1"/>
-      <c r="K46" s="1"/>
-      <c r="L46" s="1"/>
-      <c r="M46" s="1"/>
-    </row>
-    <row r="47" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="1"/>
-      <c r="B47" s="1"/>
+      <c r="L41" s="11"/>
+      <c r="M41" s="2"/>
+    </row>
+    <row r="42" customFormat="false" ht="18.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A42" s="2"/>
+      <c r="B42" s="2"/>
+      <c r="C42" s="2"/>
+      <c r="D42" s="2"/>
+      <c r="E42" s="2"/>
+      <c r="F42" s="2"/>
+      <c r="G42" s="2"/>
+      <c r="H42" s="2"/>
+      <c r="I42" s="2"/>
+      <c r="J42" s="2"/>
+      <c r="K42" s="2"/>
+      <c r="L42" s="2"/>
+      <c r="M42" s="2"/>
+    </row>
+    <row r="43" customFormat="false" ht="18.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A43" s="2"/>
+      <c r="B43" s="2"/>
+      <c r="C43" s="2"/>
+      <c r="D43" s="2"/>
+      <c r="E43" s="2"/>
+      <c r="F43" s="2"/>
+      <c r="G43" s="2"/>
+      <c r="H43" s="2"/>
+      <c r="I43" s="2"/>
+      <c r="J43" s="2"/>
+      <c r="K43" s="2"/>
+      <c r="L43" s="2"/>
+      <c r="M43" s="2"/>
+    </row>
+    <row r="44" customFormat="false" ht="18.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A44" s="2"/>
+      <c r="B44" s="2"/>
+      <c r="C44" s="2"/>
+      <c r="D44" s="2"/>
+      <c r="E44" s="2"/>
+      <c r="F44" s="2"/>
+      <c r="G44" s="2"/>
+      <c r="H44" s="2"/>
+      <c r="I44" s="2"/>
+      <c r="J44" s="2"/>
+      <c r="K44" s="2"/>
+      <c r="L44" s="2"/>
+      <c r="M44" s="2"/>
+    </row>
+    <row r="45" customFormat="false" ht="18.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A45" s="2"/>
+      <c r="B45" s="2"/>
+      <c r="C45" s="2"/>
+      <c r="D45" s="2"/>
+      <c r="E45" s="2"/>
+      <c r="F45" s="2"/>
+      <c r="G45" s="2"/>
+      <c r="H45" s="2"/>
+      <c r="I45" s="2"/>
+      <c r="J45" s="2"/>
+      <c r="K45" s="2"/>
+      <c r="L45" s="2"/>
+      <c r="M45" s="2"/>
+    </row>
+    <row r="46" customFormat="false" ht="18.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A46" s="2"/>
+      <c r="B46" s="2"/>
+      <c r="C46" s="2"/>
+      <c r="D46" s="2"/>
+      <c r="E46" s="2"/>
+      <c r="F46" s="2"/>
+      <c r="G46" s="2"/>
+      <c r="H46" s="2"/>
+      <c r="I46" s="2"/>
+      <c r="J46" s="2"/>
+      <c r="K46" s="2"/>
+      <c r="L46" s="2"/>
+      <c r="M46" s="2"/>
+    </row>
+    <row r="47" customFormat="false" ht="18.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A47" s="2"/>
+      <c r="B47" s="2"/>
       <c r="C47" s="33"/>
       <c r="D47" s="33"/>
       <c r="E47" s="33"/>
@@ -1542,13 +1542,13 @@
       <c r="H47" s="33"/>
       <c r="I47" s="33"/>
       <c r="J47" s="33"/>
-      <c r="K47" s="1"/>
-      <c r="L47" s="1"/>
-      <c r="M47" s="1"/>
-    </row>
-    <row r="48" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="1"/>
-      <c r="B48" s="1"/>
+      <c r="K47" s="2"/>
+      <c r="L47" s="2"/>
+      <c r="M47" s="2"/>
+    </row>
+    <row r="48" customFormat="false" ht="18.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A48" s="2"/>
+      <c r="B48" s="2"/>
       <c r="C48" s="33"/>
       <c r="D48" s="33"/>
       <c r="E48" s="33"/>
@@ -1557,13 +1557,13 @@
       <c r="H48" s="33"/>
       <c r="I48" s="33"/>
       <c r="J48" s="33"/>
-      <c r="K48" s="1"/>
-      <c r="L48" s="1"/>
-      <c r="M48" s="1"/>
-    </row>
-    <row r="49" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="1"/>
-      <c r="B49" s="1"/>
+      <c r="K48" s="2"/>
+      <c r="L48" s="2"/>
+      <c r="M48" s="2"/>
+    </row>
+    <row r="49" customFormat="false" ht="18.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A49" s="2"/>
+      <c r="B49" s="2"/>
       <c r="C49" s="33"/>
       <c r="D49" s="33"/>
       <c r="E49" s="33"/>
@@ -1572,13 +1572,13 @@
       <c r="H49" s="33"/>
       <c r="I49" s="33"/>
       <c r="J49" s="33"/>
-      <c r="K49" s="1"/>
-      <c r="L49" s="1"/>
-      <c r="M49" s="1"/>
-    </row>
-    <row r="50" customFormat="false" ht="13" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A50" s="1"/>
-      <c r="B50" s="1"/>
+      <c r="K49" s="2"/>
+      <c r="L49" s="2"/>
+      <c r="M49" s="2"/>
+    </row>
+    <row r="50" customFormat="false" ht="18.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A50" s="2"/>
+      <c r="B50" s="2"/>
       <c r="C50" s="33"/>
       <c r="D50" s="33"/>
       <c r="E50" s="33"/>
@@ -1587,13 +1587,13 @@
       <c r="H50" s="33"/>
       <c r="I50" s="33"/>
       <c r="J50" s="33"/>
-      <c r="K50" s="1"/>
-      <c r="L50" s="1"/>
-      <c r="M50" s="1"/>
-    </row>
-    <row r="51" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="1"/>
-      <c r="B51" s="1"/>
+      <c r="K50" s="2"/>
+      <c r="L50" s="2"/>
+      <c r="M50" s="2"/>
+    </row>
+    <row r="51" customFormat="false" ht="18.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A51" s="2"/>
+      <c r="B51" s="2"/>
       <c r="C51" s="33"/>
       <c r="D51" s="33"/>
       <c r="E51" s="33"/>
@@ -1602,13 +1602,13 @@
       <c r="H51" s="33"/>
       <c r="I51" s="33"/>
       <c r="J51" s="33"/>
-      <c r="K51" s="1"/>
-      <c r="L51" s="1"/>
-      <c r="M51" s="1"/>
-    </row>
-    <row r="52" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="1"/>
-      <c r="B52" s="1"/>
+      <c r="K51" s="2"/>
+      <c r="L51" s="2"/>
+      <c r="M51" s="2"/>
+    </row>
+    <row r="52" customFormat="false" ht="18.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A52" s="2"/>
+      <c r="B52" s="2"/>
       <c r="C52" s="33"/>
       <c r="D52" s="33"/>
       <c r="E52" s="33"/>
@@ -1617,13 +1617,13 @@
       <c r="H52" s="33"/>
       <c r="I52" s="33"/>
       <c r="J52" s="33"/>
-      <c r="K52" s="1"/>
-      <c r="L52" s="1"/>
-      <c r="M52" s="1"/>
-    </row>
-    <row r="53" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="1"/>
-      <c r="B53" s="1"/>
+      <c r="K52" s="2"/>
+      <c r="L52" s="2"/>
+      <c r="M52" s="2"/>
+    </row>
+    <row r="53" customFormat="false" ht="18.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A53" s="2"/>
+      <c r="B53" s="2"/>
       <c r="C53" s="33"/>
       <c r="D53" s="33"/>
       <c r="E53" s="33"/>
@@ -1632,32 +1632,26 @@
       <c r="H53" s="33"/>
       <c r="I53" s="33"/>
       <c r="J53" s="33"/>
-      <c r="K53" s="1"/>
-      <c r="L53" s="1"/>
-      <c r="M53" s="1"/>
-    </row>
-    <row r="54" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="1"/>
-      <c r="M54" s="1"/>
-    </row>
-    <row r="55" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="1"/>
-      <c r="M55" s="1"/>
-    </row>
-    <row r="56" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="1"/>
-      <c r="M56" s="1"/>
-    </row>
-    <row r="57" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="1"/>
-      <c r="M57" s="1"/>
-    </row>
-    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="K53" s="2"/>
+      <c r="L53" s="2"/>
+      <c r="M53" s="2"/>
+    </row>
+    <row r="54" customFormat="false" ht="18.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A54" s="2"/>
+      <c r="M54" s="2"/>
+    </row>
+    <row r="55" customFormat="false" ht="18.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A55" s="2"/>
+      <c r="M55" s="2"/>
+    </row>
+    <row r="56" customFormat="false" ht="18.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A56" s="2"/>
+      <c r="M56" s="2"/>
+    </row>
+    <row r="57" customFormat="false" ht="18.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A57" s="2"/>
+      <c r="M57" s="2"/>
+    </row>
   </sheetData>
   <mergeCells count="9">
     <mergeCell ref="B5:K5"/>

</xml_diff>

<commit_message>
update templates with a second 'Logging' sheet to save config data
</commit_message>
<xml_diff>
--- a/data/templates/template_timesheet_19_days.xlsx
+++ b/data/templates/template_timesheet_19_days.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="true"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Logging" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Timesheet" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +21,16 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
+  <si>
+    <t xml:space="preserve">carryover</t>
+  </si>
+  <si>
+    <t xml:space="preserve">row</t>
+  </si>
+  <si>
+    <t xml:space="preserve">column</t>
+  </si>
   <si>
     <t xml:space="preserve">Stundenzettel</t>
   </si>
@@ -502,9 +512,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>153360</xdr:colOff>
+      <xdr:colOff>152640</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>192240</xdr:rowOff>
+      <xdr:rowOff>191520</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -518,7 +528,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="332280" y="178200"/>
-          <a:ext cx="2477160" cy="1116360"/>
+          <a:ext cx="2476440" cy="1115640"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -536,12 +546,60 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.4"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1" s="0" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
   <dimension ref="A1:M1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12:G30"/>
+      <selection pane="topLeft" activeCell="J32" activeCellId="0" sqref="J32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.65" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -620,7 +678,7 @@
     <row r="5" customFormat="false" ht="21.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1"/>
       <c r="B5" s="2" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
@@ -653,7 +711,7 @@
       <c r="A7" s="1"/>
       <c r="B7" s="3"/>
       <c r="C7" s="4" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
@@ -670,14 +728,14 @@
       <c r="A8" s="1"/>
       <c r="B8" s="3"/>
       <c r="C8" s="4" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
       <c r="H8" s="7" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I8" s="7"/>
       <c r="J8" s="8" t="n">
@@ -706,32 +764,32 @@
       <c r="A10" s="1"/>
       <c r="B10" s="3"/>
       <c r="C10" s="4" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="K10" s="4"/>
       <c r="L10" s="9" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="M10" s="1"/>
     </row>
@@ -1230,7 +1288,7 @@
       <c r="F32" s="6"/>
       <c r="G32" s="6"/>
       <c r="H32" s="7" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I32" s="7"/>
       <c r="J32" s="27" t="n">
@@ -1290,7 +1348,7 @@
       <c r="A36" s="1"/>
       <c r="B36" s="3"/>
       <c r="C36" s="28" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D36" s="29" t="n">
         <f aca="false">ROWS(D12:D30)*8</f>
@@ -1300,7 +1358,7 @@
       <c r="F36" s="3"/>
       <c r="G36" s="3"/>
       <c r="H36" s="30" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="I36" s="29" t="n">
         <f aca="false">SUM(I12:I30)</f>
@@ -1345,19 +1403,19 @@
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D39" s="1"/>
       <c r="E39" s="1"/>
       <c r="F39" s="1"/>
       <c r="G39" s="1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="H39" s="1"/>
       <c r="I39" s="1"/>
       <c r="J39" s="1"/>
       <c r="K39" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="L39" s="1"/>
       <c r="M39" s="1"/>
@@ -1381,19 +1439,19 @@
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D41" s="1"/>
       <c r="E41" s="1"/>
       <c r="F41" s="1"/>
       <c r="G41" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="H41" s="1"/>
       <c r="I41" s="1"/>
       <c r="J41" s="1"/>
       <c r="K41" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="L41" s="1"/>
       <c r="M41" s="1"/>

</xml_diff>